<commit_message>
trabajo e chino pero yo feliz po web dice chileno prisionero
</commit_message>
<xml_diff>
--- a/assets uarm/2019 sol-penscri-justfilpol/S E B Ago2019/chronoBiSemReemp.xlsx
+++ b/assets uarm/2019 sol-penscri-justfilpol/S E B Ago2019/chronoBiSemReemp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>sab 26</t>
   </si>
@@ -77,12 +77,6 @@
     <t>crítica a la modernidad</t>
   </si>
   <si>
-    <t xml:space="preserve">Control 2: será tomado a mi </t>
-  </si>
-  <si>
-    <t>retorno, el jueves 14 de noviembre.</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=ivee1ZYdd5Y</t>
   </si>
   <si>
@@ -96,6 +90,48 @@
   </si>
   <si>
     <t>Trabajo grupal en clase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control 2: "será tomado a mi </t>
+  </si>
+  <si>
+    <t>retorno, el jueves 14 de noviembre"</t>
+  </si>
+  <si>
+    <t>unidad 6</t>
+  </si>
+  <si>
+    <t>casuistica, toma de decisiones</t>
+  </si>
+  <si>
+    <t>dilemas empresariales entre moral y pérdida</t>
+  </si>
+  <si>
+    <t>Lectura: Peter Singer 483-498</t>
+  </si>
+  <si>
+    <t>discusion de lectura, traer resumen escrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dilemas personales: pérdida </t>
+  </si>
+  <si>
+    <t>o abandono de la ética. Otros dilemas en negocios</t>
+  </si>
+  <si>
+    <t>Lectura: Paladino 12-30</t>
+  </si>
+  <si>
+    <t>lectura debatida, traer resumen</t>
+  </si>
+  <si>
+    <t>Coloquio</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>taylor - incmsrbld</t>
   </si>
 </sst>
 </file>
@@ -134,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +180,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,12 +215,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -448,17 +506,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H12"/>
+  <dimension ref="B1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" customWidth="1"/>
   </cols>
@@ -495,97 +554,187 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="7"/>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>